<commit_message>
4 and 5 clusters
</commit_message>
<xml_diff>
--- a/SHC code/sims/K_4_tetrahedron.xlsx
+++ b/SHC code/sims/K_4_tetrahedron.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steve\Documents\GitHub\thesis\SHC code\sims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927A266C-CCCE-4055-BFBC-FDB323533541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2F692A7-B319-4798-92F9-792E43684DFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9CA45C61-1169-4AC7-9660-1FA924585924}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="102">
   <si>
     <t>$|\hat{K}=K|$ (mean $\hat{K}$)</t>
   </si>
@@ -337,6 +337,9 @@
   </si>
   <si>
     <t>Median time for 1 replication (sec.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
   </si>
 </sst>
 </file>
@@ -805,7 +808,7 @@
   <dimension ref="A1:O77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -816,7 +819,7 @@
     <col min="12" max="12" width="14.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>9</v>
       </c>
@@ -837,8 +840,11 @@
         <v>100</v>
       </c>
       <c r="L1" s="10"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -876,7 +882,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>200</v>
       </c>
@@ -914,7 +920,7 @@
         <v>16.36</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>200</v>
       </c>
@@ -952,7 +958,7 @@
         <v>19.02</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>200</v>
       </c>
@@ -990,7 +996,7 @@
         <v>20.46</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>200</v>
       </c>
@@ -1028,7 +1034,7 @@
         <v>20.53</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>200</v>
       </c>
@@ -1066,7 +1072,7 @@
         <v>20.55</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>200</v>
       </c>
@@ -1104,7 +1110,7 @@
         <v>12.58</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>200</v>
       </c>
@@ -1142,7 +1148,7 @@
         <v>20.21</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>200</v>
       </c>
@@ -1180,7 +1186,7 @@
         <v>23.07</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>200</v>
       </c>
@@ -1218,7 +1224,7 @@
         <v>24.31</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>200</v>
       </c>
@@ -1256,7 +1262,7 @@
         <v>25.08</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>200</v>
       </c>
@@ -1294,7 +1300,7 @@
         <v>23.13</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>200</v>
       </c>
@@ -1332,7 +1338,7 @@
         <v>20.96</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>200</v>
       </c>
@@ -1370,7 +1376,7 @@
         <v>23.81</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>200</v>
       </c>

</xml_diff>